<commit_message>
Keep cell datatype on --append; split test file to old and new
</commit_message>
<xml_diff>
--- a/test1append.xlsx
+++ b/test1append.xlsx
@@ -4,34 +4,63 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Appended" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1-Appended" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+  </numFmts>
+  <fonts count="5">
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -48,17 +77,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -415,644 +485,529 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="6">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Example TableOld</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
-      <c r="G1" t="inlineStr"/>
-      <c r="H1" t="inlineStr"/>
-      <c r="I1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Diff test: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --out test1diff.xlsx</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Merge test: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --merge=Color --out test1merge.xlsx</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Apend test: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --append --out test1append.xlsx</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="6">
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>Diff test:  xltablediff.py  --key=ID test1old.xlsx test1new.xlsx --out test1diff.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="6">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>Merge test:  xltablediff.py  --key=ID test1old.xlsx test1new.xlsx --merge=Color --out test1merge.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="6">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>Append test:  xltablediff.py  --key=ID test1old.xlsx test1new.xlsx --append --out test1append.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6" ht="12.8" customHeight="1" s="6">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="8" t="inlineStr">
         <is>
           <t>Origin</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="8" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="G6" s="1" t="inlineStr">
+      <c r="G6" s="9" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="H6" s="1" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>Shape</t>
         </is>
       </c>
-      <c r="I6" s="1" t="inlineStr">
+      <c r="I6" s="9" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2022-11-01 00:00:00</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+    <row r="7" ht="12.8" customHeight="1" s="6">
+      <c r="A7" s="10" t="n">
+        <v>44866</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="inlineStr">
         <is>
           <t>apricot</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="8" t="inlineStr">
         <is>
           <t>Washington</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="8" t="inlineStr">
         <is>
           <t>red-orange</t>
         </is>
       </c>
-      <c r="F7" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="G7" s="1" t="inlineStr">
+      <c r="F7" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" s="9" t="inlineStr">
         <is>
           <t>apricot</t>
         </is>
       </c>
-      <c r="H7" s="1" t="inlineStr">
+      <c r="H7" s="9" t="inlineStr">
         <is>
           <t>roundish</t>
         </is>
       </c>
-      <c r="I7" s="1" t="inlineStr">
+      <c r="I7" s="9" t="inlineStr">
         <is>
           <t>red-orange</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2022-11-01 00:00:00</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+    <row r="8" ht="12.8" customHeight="1" s="6">
+      <c r="A8" s="10" t="n">
+        <v>44866</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="inlineStr">
         <is>
           <t>apple</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>Maine</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="8" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr"/>
-      <c r="G8" s="1" t="inlineStr"/>
-      <c r="H8" s="1" t="inlineStr"/>
-      <c r="I8" s="1" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2022-11-02 00:00:00</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="F8" s="9" t="n"/>
+      <c r="G8" s="9" t="n"/>
+      <c r="H8" s="9" t="n"/>
+      <c r="I8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="6">
+      <c r="A9" s="10" t="n">
+        <v>44867</v>
+      </c>
+      <c r="B9" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8" t="inlineStr">
         <is>
           <t>peach</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="8" t="inlineStr">
         <is>
           <t>Georgia</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>yellow-pink</t>
         </is>
       </c>
-      <c r="F9" s="1" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="G9" s="1" t="inlineStr">
+      <c r="F9" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" s="9" t="inlineStr">
         <is>
           <t>peach</t>
         </is>
       </c>
-      <c r="H9" s="1" t="inlineStr">
+      <c r="H9" s="9" t="inlineStr">
         <is>
           <t>roundish</t>
         </is>
       </c>
-      <c r="I9" s="1" t="inlineStr">
+      <c r="I9" s="9" t="inlineStr">
         <is>
           <t>yellow-pink</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2022-11-02 00:00:00</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
+    <row r="10" ht="12.8" customHeight="1" s="6">
+      <c r="A10" s="10" t="n">
+        <v>44867</v>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="8" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="8" t="inlineStr">
         <is>
           <t>pink</t>
         </is>
       </c>
-      <c r="F10" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G10" s="1" t="inlineStr">
+      <c r="F10" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="9" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
       </c>
-      <c r="H10" s="1" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>elongated</t>
         </is>
       </c>
-      <c r="I10" s="1" t="inlineStr">
+      <c r="I10" s="9" t="inlineStr">
         <is>
           <t>salmon</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2022-11-03 00:00:00</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
+    <row r="11" ht="12.8" customHeight="1" s="6">
+      <c r="A11" s="10" t="n">
+        <v>44868</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="inlineStr">
         <is>
           <t>plum</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="8" t="inlineStr">
         <is>
           <t>Alabama</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="8" t="inlineStr">
         <is>
           <t>purple</t>
         </is>
       </c>
-      <c r="F11" s="1" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="G11" s="1" t="inlineStr">
+      <c r="F11" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="G11" s="9" t="inlineStr">
         <is>
           <t>plum</t>
         </is>
       </c>
-      <c r="H11" s="1" t="inlineStr">
+      <c r="H11" s="9" t="inlineStr">
         <is>
           <t>round</t>
         </is>
       </c>
-      <c r="I11" s="1" t="inlineStr">
+      <c r="I11" s="9" t="inlineStr">
         <is>
           <t>purple</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2022-11-05 00:00:00</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+    <row r="12" ht="12.8" customHeight="1" s="6">
+      <c r="A12" s="10" t="n">
+        <v>44870</v>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8" t="inlineStr">
         <is>
           <t>banana</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="8" t="inlineStr">
         <is>
           <t>Chile</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="8" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
-      <c r="F12" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G12" s="1" t="inlineStr">
+      <c r="F12" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="9" t="inlineStr">
         <is>
           <t>mango</t>
         </is>
       </c>
-      <c r="H12" s="1" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>oval</t>
         </is>
       </c>
-      <c r="I12" s="1" t="inlineStr">
+      <c r="I12" s="9" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2022-11-05 00:00:00</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+    <row r="13" ht="12.8" customHeight="1" s="6">
+      <c r="A13" s="10" t="n">
+        <v>44870</v>
+      </c>
+      <c r="B13" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="8" t="inlineStr">
         <is>
           <t>pineapple</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="8" t="inlineStr">
         <is>
           <t>green-yellow</t>
         </is>
       </c>
-      <c r="F13" s="1" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="G13" s="1" t="inlineStr">
+      <c r="F13" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" s="9" t="inlineStr">
         <is>
           <t>pineapple</t>
         </is>
       </c>
-      <c r="H13" s="1" t="inlineStr">
+      <c r="H13" s="9" t="inlineStr">
         <is>
           <t>spikey</t>
         </is>
       </c>
-      <c r="I13" s="1" t="inlineStr">
+      <c r="I13" s="9" t="inlineStr">
         <is>
           <t>green-yellow</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2022-11-06 00:00:00</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
+    <row r="14" ht="12.8" customHeight="1" s="6">
+      <c r="A14" s="10" t="n">
+        <v>44871</v>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" s="8" t="inlineStr">
         <is>
           <t>tangerine</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="8" t="inlineStr">
         <is>
           <t>California</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="8" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-      <c r="F14" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="G14" s="1" t="inlineStr">
+      <c r="F14" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="9" t="inlineStr">
         <is>
           <t>tangerine</t>
         </is>
       </c>
-      <c r="H14" s="1" t="inlineStr">
+      <c r="H14" s="9" t="inlineStr">
         <is>
           <t>round</t>
         </is>
       </c>
-      <c r="I14" s="1" t="inlineStr">
+      <c r="I14" s="9" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2022-11-07 00:00:00</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
+    <row r="15" ht="12.8" customHeight="1" s="6">
+      <c r="A15" s="10" t="n">
+        <v>44872</v>
+      </c>
+      <c r="B15" s="8" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" s="8" t="inlineStr">
         <is>
           <t>persimmon</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="8" t="inlineStr">
         <is>
           <t>Iran</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="8" t="inlineStr">
         <is>
           <t>deep orange</t>
         </is>
       </c>
-      <c r="F15" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="G15" s="1" t="inlineStr">
+      <c r="F15" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="G15" s="9" t="inlineStr">
         <is>
           <t>persimmon</t>
         </is>
       </c>
-      <c r="H15" s="1" t="inlineStr">
+      <c r="H15" s="9" t="inlineStr">
         <is>
           <t>acorn</t>
         </is>
       </c>
-      <c r="I15" s="1" t="inlineStr">
+      <c r="I15" s="9" t="inlineStr">
         <is>
           <t>deep orange</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2022-11-20 00:00:00</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
+    <row r="16" ht="12.8" customHeight="1" s="6">
+      <c r="A16" s="10" t="n">
+        <v>44885</v>
+      </c>
+      <c r="B16" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="8" t="inlineStr">
         <is>
           <t>coconut</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="8" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" s="8" t="inlineStr">
         <is>
           <t>brown</t>
         </is>
       </c>
-      <c r="F16" s="1" t="inlineStr"/>
-      <c r="G16" s="1" t="inlineStr"/>
-      <c r="H16" s="1" t="inlineStr"/>
-      <c r="I16" s="1" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2022-11-21 00:00:00</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
+      <c r="F16" s="9" t="n"/>
+      <c r="G16" s="9" t="n"/>
+      <c r="H16" s="9" t="n"/>
+      <c r="I16" s="9" t="n"/>
+    </row>
+    <row r="17" ht="12.8" customHeight="1" s="6">
+      <c r="A17" s="10" t="n">
+        <v>44886</v>
+      </c>
+      <c r="B17" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="8" t="inlineStr">
         <is>
           <t>Thailand</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G17" s="1" t="inlineStr">
+      <c r="E17" s="8" t="n"/>
+      <c r="F17" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="H17" s="1" t="inlineStr">
+      <c r="H17" s="9" t="inlineStr">
         <is>
           <t>flat</t>
         </is>
       </c>
-      <c r="I17" s="1" t="inlineStr">
+      <c r="I17" s="9" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Trailing row here</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-    </row>
+      <c r="J17" s="8" t="n"/>
+    </row>
+    <row r="18" ht="12.8" customHeight="1" s="6">
+      <c r="J18" s="11" t="n"/>
+    </row>
+    <row r="19" ht="12.8" customHeight="1" s="6"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved help and tests
</commit_message>
<xml_diff>
--- a/test1append.xlsx
+++ b/test1append.xlsx
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -47,6 +47,11 @@
       <family val="2"/>
       <b val="1"/>
       <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="4">
@@ -87,7 +92,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -95,6 +100,9 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -111,6 +119,9 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -492,511 +503,526 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="6">
-      <c r="A1" s="7" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="7">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Example TableOld</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="6">
-      <c r="A2" s="8" t="inlineStr">
-        <is>
-          <t>Diff test:  xltablediff.py  --key=ID test1old.xlsx test1new.xlsx --out test1diff.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="12.8" customHeight="1" s="6">
-      <c r="A3" s="8" t="inlineStr">
-        <is>
-          <t>Merge test:  xltablediff.py  --key=ID test1old.xlsx test1new.xlsx --merge=Color --out test1merge.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="12.8" customHeight="1" s="6">
-      <c r="A4" s="8" t="inlineStr">
-        <is>
-          <t>Append test:  xltablediff.py  --key=ID test1old.xlsx test1new.xlsx --append --out test1append.xlsx</t>
+    <row r="2" ht="12.8" customHeight="1" s="7">
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>Diff test:</t>
+        </is>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>xltablediff.py  --key ID test1old.xlsx test1new.xlsx --out test1diff.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="7">
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t>Merge test:</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>xltablediff.py  --key ID --merge Color test1old.xlsx test1new.xlsx --out test1merge.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="7">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Append test:</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>xltablediff.py  --key ID --append test1old.xlsx test1new.xlsx --out test1append.xlsx</t>
         </is>
       </c>
     </row>
     <row r="5"/>
-    <row r="6" ht="12.8" customHeight="1" s="6">
-      <c r="A6" s="8" t="inlineStr">
+    <row r="6" ht="12.8" customHeight="1" s="7">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B6" s="8" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C6" s="8" t="inlineStr">
+      <c r="C6" s="9" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="D6" s="8" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>Origin</t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="E6" s="9" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
-      <c r="F6" s="9" t="inlineStr">
+      <c r="F6" s="11" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="G6" s="9" t="inlineStr">
+      <c r="G6" s="11" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="H6" s="9" t="inlineStr">
+      <c r="H6" s="11" t="inlineStr">
         <is>
           <t>Shape</t>
         </is>
       </c>
-      <c r="I6" s="9" t="inlineStr">
+      <c r="I6" s="11" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="12.8" customHeight="1" s="6">
-      <c r="A7" s="10" t="n">
+    <row r="7" ht="12.8" customHeight="1" s="7">
+      <c r="A7" s="12" t="n">
         <v>44866</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="C7" s="8" t="inlineStr">
+      <c r="C7" s="9" t="inlineStr">
         <is>
           <t>apricot</t>
         </is>
       </c>
-      <c r="D7" s="8" t="inlineStr">
+      <c r="D7" s="9" t="inlineStr">
         <is>
           <t>Washington</t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr">
+      <c r="E7" s="9" t="inlineStr">
         <is>
           <t>red-orange</t>
         </is>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="G7" s="9" t="inlineStr">
+      <c r="G7" s="11" t="inlineStr">
         <is>
           <t>apricot</t>
         </is>
       </c>
-      <c r="H7" s="9" t="inlineStr">
+      <c r="H7" s="11" t="inlineStr">
         <is>
           <t>roundish</t>
         </is>
       </c>
-      <c r="I7" s="9" t="inlineStr">
+      <c r="I7" s="11" t="inlineStr">
         <is>
           <t>red-orange</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="12.8" customHeight="1" s="6">
-      <c r="A8" s="10" t="n">
+    <row r="8" ht="12.8" customHeight="1" s="7">
+      <c r="A8" s="12" t="n">
         <v>44866</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="inlineStr">
+      <c r="C8" s="9" t="inlineStr">
         <is>
           <t>apple</t>
         </is>
       </c>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>Maine</t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="9" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="F8" s="9" t="n"/>
-      <c r="G8" s="9" t="n"/>
-      <c r="H8" s="9" t="n"/>
-      <c r="I8" s="9" t="n"/>
-    </row>
-    <row r="9" ht="12.8" customHeight="1" s="6">
-      <c r="A9" s="10" t="n">
+      <c r="F8" s="11" t="n"/>
+      <c r="G8" s="11" t="n"/>
+      <c r="H8" s="11" t="n"/>
+      <c r="I8" s="11" t="n"/>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="7">
+      <c r="A9" s="12" t="n">
         <v>44867</v>
       </c>
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="8" t="inlineStr">
+      <c r="C9" s="9" t="inlineStr">
         <is>
           <t>peach</t>
         </is>
       </c>
-      <c r="D9" s="8" t="inlineStr">
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>Georgia</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
+      <c r="E9" s="9" t="inlineStr">
         <is>
           <t>yellow-pink</t>
         </is>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="9" t="inlineStr">
+      <c r="G9" s="11" t="inlineStr">
         <is>
           <t>peach</t>
         </is>
       </c>
-      <c r="H9" s="9" t="inlineStr">
+      <c r="H9" s="11" t="inlineStr">
         <is>
           <t>roundish</t>
         </is>
       </c>
-      <c r="I9" s="9" t="inlineStr">
+      <c r="I9" s="11" t="inlineStr">
         <is>
           <t>yellow-pink</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="12.8" customHeight="1" s="6">
-      <c r="A10" s="10" t="n">
+    <row r="10" ht="12.8" customHeight="1" s="7">
+      <c r="A10" s="12" t="n">
         <v>44867</v>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="8" t="inlineStr">
+      <c r="C10" s="9" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
       </c>
-      <c r="D10" s="8" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>pink</t>
         </is>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="G10" s="9" t="inlineStr">
+      <c r="G10" s="11" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
       </c>
-      <c r="H10" s="9" t="inlineStr">
+      <c r="H10" s="11" t="inlineStr">
         <is>
           <t>elongated</t>
         </is>
       </c>
-      <c r="I10" s="9" t="inlineStr">
+      <c r="I10" s="11" t="inlineStr">
         <is>
           <t>salmon</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="12.8" customHeight="1" s="6">
-      <c r="A11" s="10" t="n">
+    <row r="11" ht="12.8" customHeight="1" s="7">
+      <c r="A11" s="12" t="n">
         <v>44868</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="inlineStr">
+      <c r="C11" s="9" t="inlineStr">
         <is>
           <t>plum</t>
         </is>
       </c>
-      <c r="D11" s="8" t="inlineStr">
+      <c r="D11" s="9" t="inlineStr">
         <is>
           <t>Alabama</t>
         </is>
       </c>
-      <c r="E11" s="8" t="inlineStr">
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>purple</t>
         </is>
       </c>
-      <c r="F11" s="9" t="n">
+      <c r="F11" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="G11" s="9" t="inlineStr">
+      <c r="G11" s="11" t="inlineStr">
         <is>
           <t>plum</t>
         </is>
       </c>
-      <c r="H11" s="9" t="inlineStr">
+      <c r="H11" s="11" t="inlineStr">
         <is>
           <t>round</t>
         </is>
       </c>
-      <c r="I11" s="9" t="inlineStr">
+      <c r="I11" s="11" t="inlineStr">
         <is>
           <t>purple</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="12.8" customHeight="1" s="6">
-      <c r="A12" s="10" t="n">
+    <row r="12" ht="12.8" customHeight="1" s="7">
+      <c r="A12" s="12" t="n">
         <v>44870</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="8" t="inlineStr">
+      <c r="C12" s="9" t="inlineStr">
         <is>
           <t>banana</t>
         </is>
       </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>Chile</t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="E12" s="9" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
-      <c r="F12" s="9" t="n">
+      <c r="F12" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="9" t="inlineStr">
+      <c r="G12" s="11" t="inlineStr">
         <is>
           <t>mango</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
+      <c r="H12" s="11" t="inlineStr">
         <is>
           <t>oval</t>
         </is>
       </c>
-      <c r="I12" s="9" t="inlineStr">
+      <c r="I12" s="11" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="12.8" customHeight="1" s="6">
-      <c r="A13" s="10" t="n">
+    <row r="13" ht="12.8" customHeight="1" s="7">
+      <c r="A13" s="12" t="n">
         <v>44870</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="inlineStr">
+      <c r="C13" s="9" t="inlineStr">
         <is>
           <t>pineapple</t>
         </is>
       </c>
-      <c r="D13" s="8" t="inlineStr">
+      <c r="D13" s="9" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="E13" s="8" t="inlineStr">
+      <c r="E13" s="9" t="inlineStr">
         <is>
           <t>green-yellow</t>
         </is>
       </c>
-      <c r="F13" s="9" t="n">
+      <c r="F13" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="G13" s="9" t="inlineStr">
+      <c r="G13" s="11" t="inlineStr">
         <is>
           <t>pineapple</t>
         </is>
       </c>
-      <c r="H13" s="9" t="inlineStr">
+      <c r="H13" s="11" t="inlineStr">
         <is>
           <t>spikey</t>
         </is>
       </c>
-      <c r="I13" s="9" t="inlineStr">
+      <c r="I13" s="11" t="inlineStr">
         <is>
           <t>green-yellow</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="12.8" customHeight="1" s="6">
-      <c r="A14" s="10" t="n">
+    <row r="14" ht="12.8" customHeight="1" s="7">
+      <c r="A14" s="12" t="n">
         <v>44871</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C14" s="8" t="inlineStr">
+      <c r="C14" s="9" t="inlineStr">
         <is>
           <t>tangerine</t>
         </is>
       </c>
-      <c r="D14" s="8" t="inlineStr">
+      <c r="D14" s="9" t="inlineStr">
         <is>
           <t>California</t>
         </is>
       </c>
-      <c r="E14" s="8" t="inlineStr">
+      <c r="E14" s="9" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-      <c r="F14" s="9" t="n">
+      <c r="F14" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="G14" s="9" t="inlineStr">
+      <c r="G14" s="11" t="inlineStr">
         <is>
           <t>tangerine</t>
         </is>
       </c>
-      <c r="H14" s="9" t="inlineStr">
+      <c r="H14" s="11" t="inlineStr">
         <is>
           <t>round</t>
         </is>
       </c>
-      <c r="I14" s="9" t="inlineStr">
+      <c r="I14" s="11" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="12.8" customHeight="1" s="6">
-      <c r="A15" s="10" t="n">
+    <row r="15" ht="12.8" customHeight="1" s="7">
+      <c r="A15" s="12" t="n">
         <v>44872</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="8" t="inlineStr">
+      <c r="C15" s="9" t="inlineStr">
         <is>
           <t>persimmon</t>
         </is>
       </c>
-      <c r="D15" s="8" t="inlineStr">
+      <c r="D15" s="9" t="inlineStr">
         <is>
           <t>Iran</t>
         </is>
       </c>
-      <c r="E15" s="8" t="inlineStr">
+      <c r="E15" s="9" t="inlineStr">
         <is>
           <t>deep orange</t>
         </is>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="G15" s="9" t="inlineStr">
+      <c r="G15" s="11" t="inlineStr">
         <is>
           <t>persimmon</t>
         </is>
       </c>
-      <c r="H15" s="9" t="inlineStr">
+      <c r="H15" s="11" t="inlineStr">
         <is>
           <t>acorn</t>
         </is>
       </c>
-      <c r="I15" s="9" t="inlineStr">
+      <c r="I15" s="11" t="inlineStr">
         <is>
           <t>deep orange</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="12.8" customHeight="1" s="6">
-      <c r="A16" s="10" t="n">
+    <row r="16" ht="12.8" customHeight="1" s="7">
+      <c r="A16" s="12" t="n">
         <v>44885</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="8" t="inlineStr">
+      <c r="C16" s="9" t="inlineStr">
         <is>
           <t>coconut</t>
         </is>
       </c>
-      <c r="D16" s="8" t="inlineStr">
+      <c r="D16" s="9" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="E16" s="8" t="inlineStr">
+      <c r="E16" s="9" t="inlineStr">
         <is>
           <t>brown</t>
         </is>
       </c>
-      <c r="F16" s="9" t="n"/>
-      <c r="G16" s="9" t="n"/>
-      <c r="H16" s="9" t="n"/>
-      <c r="I16" s="9" t="n"/>
-    </row>
-    <row r="17" ht="12.8" customHeight="1" s="6">
-      <c r="A17" s="10" t="n">
+      <c r="F16" s="11" t="n"/>
+      <c r="G16" s="11" t="n"/>
+      <c r="H16" s="11" t="n"/>
+      <c r="I16" s="11" t="n"/>
+    </row>
+    <row r="17" ht="12.8" customHeight="1" s="7">
+      <c r="A17" s="12" t="n">
         <v>44886</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C17" s="8" t="inlineStr">
+      <c r="C17" s="9" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="D17" s="8" t="inlineStr">
+      <c r="D17" s="9" t="inlineStr">
         <is>
           <t>Thailand</t>
         </is>
       </c>
-      <c r="E17" s="8" t="n"/>
-      <c r="F17" s="9" t="n">
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="G17" s="9" t="inlineStr">
+      <c r="G17" s="11" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="H17" s="9" t="inlineStr">
+      <c r="H17" s="11" t="inlineStr">
         <is>
           <t>flat</t>
         </is>
       </c>
-      <c r="I17" s="9" t="inlineStr">
+      <c r="I17" s="11" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-    </row>
-    <row r="18" ht="12.8" customHeight="1" s="6">
-      <c r="J18" s="11" t="n"/>
-    </row>
-    <row r="19" ht="12.8" customHeight="1" s="6"/>
+      <c r="J17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="12.8" customHeight="1" s="7">
+      <c r="J18" s="13" t="n"/>
+    </row>
+    <row r="19" ht="12.8" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added 'key OLDKEY=NEWKEY option'
</commit_message>
<xml_diff>
--- a/test1append.xlsx
+++ b/test1append.xlsx
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -47,11 +47,6 @@
       <family val="2"/>
       <b val="1"/>
       <sz val="12"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="4">
@@ -92,7 +87,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -100,9 +95,6 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -119,9 +111,6 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -500,529 +489,541 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="7">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="6">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Example TableOld</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="7">
-      <c r="A2" s="9" t="inlineStr">
+    <row r="2" ht="12.8" customHeight="1" s="6">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Diff test:</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>xltablediff.py  --key ID test1old.xlsx test1new.xlsx --out test1diff.xlsx</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="7">
-      <c r="A3" s="9" t="inlineStr">
+    <row r="3" ht="12.8" customHeight="1" s="6">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>Ignore test:</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>xltablediff.py  --key ID --ignore Color test1old.xlsx test1new.xlsx --out test1ignore.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="6">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>Merge test:</t>
         </is>
       </c>
-      <c r="B3" s="10" t="inlineStr">
+      <c r="B4" s="8" t="inlineStr">
         <is>
           <t>xltablediff.py  --key ID --merge Color test1old.xlsx test1new.xlsx --out test1merge.xlsx</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="1" s="7">
-      <c r="A4" s="9" t="inlineStr">
+    <row r="5" ht="12.8" customHeight="1" s="6">
+      <c r="A5" s="8" t="inlineStr">
         <is>
           <t>Append test:</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>xltablediff.py  --key ID --append test1old.xlsx test1new.xlsx --out test1append.xlsx</t>
         </is>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6" ht="12.8" customHeight="1" s="7">
-      <c r="A6" s="9" t="inlineStr">
+    <row r="6"/>
+    <row r="7" ht="12.8" customHeight="1" s="6">
+      <c r="A7" s="8" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="C7" s="8" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
+      <c r="D7" s="8" t="inlineStr">
         <is>
           <t>Origin</t>
         </is>
       </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="E7" s="8" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr">
+      <c r="F7" s="9" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="G6" s="11" t="inlineStr">
+      <c r="G7" s="9" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="H6" s="11" t="inlineStr">
+      <c r="H7" s="9" t="inlineStr">
         <is>
           <t>Shape</t>
         </is>
       </c>
-      <c r="I6" s="11" t="inlineStr">
+      <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="12.8" customHeight="1" s="7">
-      <c r="A7" s="12" t="n">
+    <row r="8" ht="12.8" customHeight="1" s="6">
+      <c r="A8" s="10" t="n">
         <v>44866</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B8" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="C8" s="8" t="inlineStr">
         <is>
           <t>apricot</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>Washington</t>
         </is>
       </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="E8" s="8" t="inlineStr">
         <is>
           <t>red-orange</t>
         </is>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="F8" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="G7" s="11" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>apricot</t>
         </is>
       </c>
-      <c r="H7" s="11" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>roundish</t>
         </is>
       </c>
-      <c r="I7" s="11" t="inlineStr">
+      <c r="I8" s="9" t="inlineStr">
         <is>
           <t>red-orange</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="12.8" customHeight="1" s="7">
-      <c r="A8" s="12" t="n">
+    <row r="9" ht="12.8" customHeight="1" s="6">
+      <c r="A9" s="10" t="n">
         <v>44866</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B9" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="C9" s="8" t="inlineStr">
         <is>
           <t>apple</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
+      <c r="D9" s="8" t="inlineStr">
         <is>
           <t>Maine</t>
         </is>
       </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="F8" s="11" t="n"/>
-      <c r="G8" s="11" t="n"/>
-      <c r="H8" s="11" t="n"/>
-      <c r="I8" s="11" t="n"/>
-    </row>
-    <row r="9" ht="12.8" customHeight="1" s="7">
-      <c r="A9" s="12" t="n">
+      <c r="F9" s="9" t="n"/>
+      <c r="G9" s="9" t="n"/>
+      <c r="H9" s="9" t="n"/>
+      <c r="I9" s="9" t="n"/>
+    </row>
+    <row r="10" ht="12.8" customHeight="1" s="6">
+      <c r="A10" s="10" t="n">
         <v>44867</v>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="B10" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="C10" s="8" t="inlineStr">
         <is>
           <t>peach</t>
         </is>
       </c>
-      <c r="D9" s="9" t="inlineStr">
+      <c r="D10" s="8" t="inlineStr">
         <is>
           <t>Georgia</t>
         </is>
       </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="E10" s="8" t="inlineStr">
         <is>
           <t>yellow-pink</t>
         </is>
       </c>
-      <c r="F9" s="11" t="n">
+      <c r="F10" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="11" t="inlineStr">
+      <c r="G10" s="9" t="inlineStr">
         <is>
           <t>peach</t>
         </is>
       </c>
-      <c r="H9" s="11" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>roundish</t>
         </is>
       </c>
-      <c r="I9" s="11" t="inlineStr">
+      <c r="I10" s="9" t="inlineStr">
         <is>
           <t>yellow-pink</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="12.8" customHeight="1" s="7">
-      <c r="A10" s="12" t="n">
+    <row r="11" ht="12.8" customHeight="1" s="6">
+      <c r="A11" s="10" t="n">
         <v>44867</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B11" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C11" s="8" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
+      <c r="D11" s="8" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
       </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="E11" s="8" t="inlineStr">
         <is>
           <t>pink</t>
         </is>
       </c>
-      <c r="F10" s="11" t="n">
+      <c r="F11" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G10" s="11" t="inlineStr">
+      <c r="G11" s="9" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
       </c>
-      <c r="H10" s="11" t="inlineStr">
+      <c r="H11" s="9" t="inlineStr">
         <is>
           <t>elongated</t>
         </is>
       </c>
-      <c r="I10" s="11" t="inlineStr">
+      <c r="I11" s="9" t="inlineStr">
         <is>
           <t>salmon</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="12.8" customHeight="1" s="7">
-      <c r="A11" s="12" t="n">
+    <row r="12" ht="12.8" customHeight="1" s="6">
+      <c r="A12" s="10" t="n">
         <v>44868</v>
       </c>
-      <c r="B11" s="9" t="n">
+      <c r="B12" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="9" t="inlineStr">
+      <c r="C12" s="8" t="inlineStr">
         <is>
           <t>plum</t>
         </is>
       </c>
-      <c r="D11" s="9" t="inlineStr">
+      <c r="D12" s="8" t="inlineStr">
         <is>
           <t>Alabama</t>
         </is>
       </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="E12" s="8" t="inlineStr">
         <is>
           <t>purple</t>
         </is>
       </c>
-      <c r="F11" s="11" t="n">
+      <c r="F12" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="G11" s="11" t="inlineStr">
+      <c r="G12" s="9" t="inlineStr">
         <is>
           <t>plum</t>
         </is>
       </c>
-      <c r="H11" s="11" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>round</t>
         </is>
       </c>
-      <c r="I11" s="11" t="inlineStr">
+      <c r="I12" s="9" t="inlineStr">
         <is>
           <t>purple</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="12.8" customHeight="1" s="7">
-      <c r="A12" s="12" t="n">
+    <row r="13" ht="12.8" customHeight="1" s="6">
+      <c r="A13" s="10" t="n">
         <v>44870</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="C13" s="8" t="inlineStr">
         <is>
           <t>banana</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Chile</t>
         </is>
       </c>
-      <c r="E12" s="9" t="inlineStr">
+      <c r="E13" s="8" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
-      <c r="F12" s="11" t="n">
+      <c r="F13" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="11" t="inlineStr">
+      <c r="G13" s="9" t="inlineStr">
         <is>
           <t>mango</t>
         </is>
       </c>
-      <c r="H12" s="11" t="inlineStr">
+      <c r="H13" s="9" t="inlineStr">
         <is>
           <t>oval</t>
         </is>
       </c>
-      <c r="I12" s="11" t="inlineStr">
+      <c r="I13" s="9" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="12.8" customHeight="1" s="7">
-      <c r="A13" s="12" t="n">
+    <row r="14" ht="12.8" customHeight="1" s="6">
+      <c r="A14" s="10" t="n">
         <v>44870</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="B14" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="C13" s="9" t="inlineStr">
+      <c r="C14" s="8" t="inlineStr">
         <is>
           <t>pineapple</t>
         </is>
       </c>
-      <c r="D13" s="9" t="inlineStr">
+      <c r="D14" s="8" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="E14" s="8" t="inlineStr">
         <is>
           <t>green-yellow</t>
         </is>
       </c>
-      <c r="F13" s="11" t="n">
+      <c r="F14" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="G13" s="11" t="inlineStr">
+      <c r="G14" s="9" t="inlineStr">
         <is>
           <t>pineapple</t>
         </is>
       </c>
-      <c r="H13" s="11" t="inlineStr">
+      <c r="H14" s="9" t="inlineStr">
         <is>
           <t>spikey</t>
         </is>
       </c>
-      <c r="I13" s="11" t="inlineStr">
+      <c r="I14" s="9" t="inlineStr">
         <is>
           <t>green-yellow</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="12.8" customHeight="1" s="7">
-      <c r="A14" s="12" t="n">
+    <row r="15" ht="12.8" customHeight="1" s="6">
+      <c r="A15" s="10" t="n">
         <v>44871</v>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B15" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="C14" s="9" t="inlineStr">
+      <c r="C15" s="8" t="inlineStr">
         <is>
           <t>tangerine</t>
         </is>
       </c>
-      <c r="D14" s="9" t="inlineStr">
+      <c r="D15" s="8" t="inlineStr">
         <is>
           <t>California</t>
         </is>
       </c>
-      <c r="E14" s="9" t="inlineStr">
+      <c r="E15" s="8" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-      <c r="F14" s="11" t="n">
+      <c r="F15" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="G14" s="11" t="inlineStr">
+      <c r="G15" s="9" t="inlineStr">
         <is>
           <t>tangerine</t>
         </is>
       </c>
-      <c r="H14" s="11" t="inlineStr">
+      <c r="H15" s="9" t="inlineStr">
         <is>
           <t>round</t>
         </is>
       </c>
-      <c r="I14" s="11" t="inlineStr">
+      <c r="I15" s="9" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="12.8" customHeight="1" s="7">
-      <c r="A15" s="12" t="n">
+    <row r="16" ht="12.8" customHeight="1" s="6">
+      <c r="A16" s="10" t="n">
         <v>44872</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B16" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="9" t="inlineStr">
+      <c r="C16" s="8" t="inlineStr">
         <is>
           <t>persimmon</t>
         </is>
       </c>
-      <c r="D15" s="9" t="inlineStr">
+      <c r="D16" s="8" t="inlineStr">
         <is>
           <t>Iran</t>
         </is>
       </c>
-      <c r="E15" s="9" t="inlineStr">
+      <c r="E16" s="8" t="inlineStr">
         <is>
           <t>deep orange</t>
         </is>
       </c>
-      <c r="F15" s="11" t="n">
+      <c r="F16" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="G15" s="11" t="inlineStr">
+      <c r="G16" s="9" t="inlineStr">
         <is>
           <t>persimmon</t>
         </is>
       </c>
-      <c r="H15" s="11" t="inlineStr">
+      <c r="H16" s="9" t="inlineStr">
         <is>
           <t>acorn</t>
         </is>
       </c>
-      <c r="I15" s="11" t="inlineStr">
+      <c r="I16" s="9" t="inlineStr">
         <is>
           <t>deep orange</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="12.8" customHeight="1" s="7">
-      <c r="A16" s="12" t="n">
+    <row r="17" ht="12.8" customHeight="1" s="6">
+      <c r="A17" s="10" t="n">
         <v>44885</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B17" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="9" t="inlineStr">
+      <c r="C17" s="8" t="inlineStr">
         <is>
           <t>coconut</t>
         </is>
       </c>
-      <c r="D16" s="9" t="inlineStr">
+      <c r="D17" s="8" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="E16" s="9" t="inlineStr">
+      <c r="E17" s="8" t="inlineStr">
         <is>
           <t>brown</t>
         </is>
       </c>
-      <c r="F16" s="11" t="n"/>
-      <c r="G16" s="11" t="n"/>
-      <c r="H16" s="11" t="n"/>
-      <c r="I16" s="11" t="n"/>
-    </row>
-    <row r="17" ht="12.8" customHeight="1" s="7">
-      <c r="A17" s="12" t="n">
+      <c r="F17" s="9" t="n"/>
+      <c r="G17" s="9" t="n"/>
+      <c r="H17" s="9" t="n"/>
+      <c r="I17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="12.8" customHeight="1" s="6">
+      <c r="A18" s="10" t="n">
         <v>44886</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B18" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="C17" s="9" t="inlineStr">
+      <c r="C18" s="8" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="D17" s="9" t="inlineStr">
+      <c r="D18" s="8" t="inlineStr">
         <is>
           <t>Thailand</t>
         </is>
       </c>
-      <c r="E17" s="9" t="n"/>
-      <c r="F17" s="11" t="n">
+      <c r="E18" s="8" t="n"/>
+      <c r="F18" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="G17" s="11" t="inlineStr">
+      <c r="G18" s="9" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="H17" s="11" t="inlineStr">
+      <c r="H18" s="9" t="inlineStr">
         <is>
           <t>flat</t>
         </is>
       </c>
-      <c r="I17" s="11" t="inlineStr">
+      <c r="I18" s="9" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-      <c r="J17" s="9" t="n"/>
-    </row>
-    <row r="18" ht="12.8" customHeight="1" s="7">
-      <c r="J18" s="13" t="n"/>
-    </row>
-    <row r="19" ht="12.8" customHeight="1" s="7"/>
+      <c r="J18" s="8" t="n"/>
+    </row>
+    <row r="19" ht="12.8" customHeight="1" s="6">
+      <c r="J19" s="11" t="n"/>
+    </row>
+    <row r="20" ht="12.8" customHeight="1" s="6"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Copy fills when appending
</commit_message>
<xml_diff>
--- a/test1append.xlsx
+++ b/test1append.xlsx
@@ -49,12 +49,18 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDF7CAA"/>
+        <bgColor rgb="FFFF99CC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -64,7 +70,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DDFFE2"/>
+        <fgColor rgb="00B6FFC1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC82"/>
+        <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -87,7 +99,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -104,6 +116,9 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -113,10 +128,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -131,70 +147,62 @@
   </cellStyles>
   <colors>
     <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFDF7CAA"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -489,541 +497,544 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:B3"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="6">
-      <c r="A1" s="7" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="7">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Example TableOld</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="6">
-      <c r="A2" s="8" t="inlineStr">
+    <row r="2" ht="12.8" customHeight="1" s="7">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Diff test:</t>
         </is>
       </c>
-      <c r="B2" s="8" t="inlineStr">
+      <c r="B2" s="9" t="inlineStr">
         <is>
           <t>xltablediff.py  --key ID test1old.xlsx test1new.xlsx --out test1diff.xlsx</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="6">
-      <c r="A3" s="8" t="inlineStr">
+    <row r="3" ht="12.8" customHeight="1" s="7">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>Ignore test:</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
         <is>
           <t>xltablediff.py  --key ID --ignore Color test1old.xlsx test1new.xlsx --out test1ignore.xlsx</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="1" s="6">
-      <c r="A4" s="8" t="inlineStr">
+    <row r="4" ht="12.8" customHeight="1" s="7">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>Merge test:</t>
         </is>
       </c>
-      <c r="B4" s="8" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
         <is>
           <t>xltablediff.py  --key ID --merge Color test1old.xlsx test1new.xlsx --out test1merge.xlsx</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="12.8" customHeight="1" s="6">
-      <c r="A5" s="8" t="inlineStr">
+    <row r="5" ht="12.8" customHeight="1" s="7">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>Append test:</t>
         </is>
       </c>
-      <c r="B5" s="8" t="inlineStr">
+      <c r="B5" s="9" t="inlineStr">
         <is>
           <t>xltablediff.py  --key ID --append test1old.xlsx test1new.xlsx --out test1append.xlsx</t>
         </is>
       </c>
     </row>
     <row r="6"/>
-    <row r="7" ht="12.8" customHeight="1" s="6">
-      <c r="A7" s="8" t="inlineStr">
+    <row r="7" ht="12.8" customHeight="1" s="7">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B7" s="8" t="inlineStr">
+      <c r="B7" s="9" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C7" s="8" t="inlineStr">
+      <c r="C7" s="9" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="D7" s="8" t="inlineStr">
+      <c r="D7" s="9" t="inlineStr">
         <is>
           <t>Origin</t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr">
+      <c r="E7" s="9" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
-      <c r="F7" s="9" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="G7" s="9" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="H7" s="9" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Shape</t>
         </is>
       </c>
-      <c r="I7" s="9" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="12.8" customHeight="1" s="6">
+    <row r="8" ht="12.8" customHeight="1" s="7">
       <c r="A8" s="10" t="n">
         <v>44866</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="inlineStr">
+      <c r="C8" s="9" t="inlineStr">
         <is>
           <t>apricot</t>
         </is>
       </c>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>Washington</t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="9" t="inlineStr">
         <is>
           <t>red-orange</t>
         </is>
       </c>
-      <c r="F8" s="9" t="n">
+      <c r="F8" t="n">
         <v>7</v>
       </c>
-      <c r="G8" s="9" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>apricot</t>
         </is>
       </c>
-      <c r="H8" s="9" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>roundish</t>
         </is>
       </c>
-      <c r="I8" s="9" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>red-orange</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="12.8" customHeight="1" s="6">
+    <row r="9" ht="12.8" customHeight="1" s="7">
       <c r="A9" s="10" t="n">
         <v>44866</v>
       </c>
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="inlineStr">
+      <c r="C9" s="9" t="inlineStr">
         <is>
           <t>apple</t>
         </is>
       </c>
-      <c r="D9" s="8" t="inlineStr">
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>Maine</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
+      <c r="E9" s="9" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="F9" s="9" t="n"/>
-      <c r="G9" s="9" t="n"/>
-      <c r="H9" s="9" t="n"/>
-      <c r="I9" s="9" t="n"/>
-    </row>
-    <row r="10" ht="12.8" customHeight="1" s="6">
+      <c r="F9" s="11" t="n"/>
+      <c r="G9" s="11" t="n"/>
+      <c r="H9" s="11" t="n"/>
+      <c r="I9" s="11" t="n"/>
+    </row>
+    <row r="10" ht="12.8" customHeight="1" s="7">
       <c r="A10" s="10" t="n">
         <v>44867</v>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="8" t="inlineStr">
+      <c r="C10" s="9" t="inlineStr">
         <is>
           <t>peach</t>
         </is>
       </c>
-      <c r="D10" s="8" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>Georgia</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>yellow-pink</t>
         </is>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" t="n">
         <v>8</v>
       </c>
-      <c r="G10" s="9" t="inlineStr">
+      <c r="G10" s="12" t="inlineStr">
         <is>
           <t>peach</t>
         </is>
       </c>
-      <c r="H10" s="9" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>roundish</t>
         </is>
       </c>
-      <c r="I10" s="9" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>yellow-pink</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="12.8" customHeight="1" s="6">
+    <row r="11" ht="12.8" customHeight="1" s="7">
       <c r="A11" s="10" t="n">
         <v>44867</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="8" t="inlineStr">
+      <c r="C11" s="9" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
       </c>
-      <c r="D11" s="8" t="inlineStr">
+      <c r="D11" s="9" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
       </c>
-      <c r="E11" s="8" t="inlineStr">
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>pink</t>
         </is>
       </c>
-      <c r="F11" s="9" t="n">
+      <c r="F11" t="n">
         <v>5</v>
       </c>
-      <c r="G11" s="9" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
       </c>
-      <c r="H11" s="9" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>elongated</t>
         </is>
       </c>
-      <c r="I11" s="9" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>salmon</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="12.8" customHeight="1" s="6">
+    <row r="12" ht="12.8" customHeight="1" s="7">
       <c r="A12" s="10" t="n">
         <v>44868</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="C12" s="8" t="inlineStr">
+      <c r="C12" s="13" t="inlineStr">
         <is>
           <t>plum</t>
         </is>
       </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>Alabama</t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="E12" s="9" t="inlineStr">
         <is>
           <t>purple</t>
         </is>
       </c>
-      <c r="F12" s="9" t="n">
+      <c r="F12" t="n">
         <v>9</v>
       </c>
-      <c r="G12" s="9" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>plum</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>round</t>
         </is>
       </c>
-      <c r="I12" s="9" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>purple</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="12.8" customHeight="1" s="6">
+    <row r="13" ht="12.8" customHeight="1" s="7">
       <c r="A13" s="10" t="n">
         <v>44870</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="8" t="inlineStr">
+      <c r="C13" s="9" t="inlineStr">
         <is>
           <t>banana</t>
         </is>
       </c>
-      <c r="D13" s="8" t="inlineStr">
+      <c r="D13" s="9" t="inlineStr">
         <is>
           <t>Chile</t>
         </is>
       </c>
-      <c r="E13" s="8" t="inlineStr">
+      <c r="E13" s="9" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
-      <c r="F13" s="9" t="n">
+      <c r="F13" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="9" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>mango</t>
         </is>
       </c>
-      <c r="H13" s="9" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>oval</t>
         </is>
       </c>
-      <c r="I13" s="9" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="12.8" customHeight="1" s="6">
+    <row r="14" ht="12.8" customHeight="1" s="7">
       <c r="A14" s="10" t="n">
         <v>44870</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="C14" s="8" t="inlineStr">
+      <c r="C14" s="9" t="inlineStr">
         <is>
           <t>pineapple</t>
         </is>
       </c>
-      <c r="D14" s="8" t="inlineStr">
+      <c r="D14" s="9" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="E14" s="8" t="inlineStr">
+      <c r="E14" s="9" t="inlineStr">
         <is>
           <t>green-yellow</t>
         </is>
       </c>
-      <c r="F14" s="9" t="n">
+      <c r="F14" t="n">
         <v>10</v>
       </c>
-      <c r="G14" s="9" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>pineapple</t>
         </is>
       </c>
-      <c r="H14" s="9" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>spikey</t>
         </is>
       </c>
-      <c r="I14" s="9" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>green-yellow</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="12.8" customHeight="1" s="6">
+    <row r="15" ht="12.8" customHeight="1" s="7">
       <c r="A15" s="10" t="n">
         <v>44871</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C15" s="8" t="inlineStr">
+      <c r="C15" s="9" t="inlineStr">
         <is>
           <t>tangerine</t>
         </is>
       </c>
-      <c r="D15" s="8" t="inlineStr">
+      <c r="D15" s="9" t="inlineStr">
         <is>
           <t>California</t>
         </is>
       </c>
-      <c r="E15" s="8" t="inlineStr">
+      <c r="E15" s="9" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" t="n">
         <v>6</v>
       </c>
-      <c r="G15" s="9" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>tangerine</t>
         </is>
       </c>
-      <c r="H15" s="9" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>round</t>
         </is>
       </c>
-      <c r="I15" s="9" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="12.8" customHeight="1" s="6">
+    <row r="16" ht="12.8" customHeight="1" s="7">
       <c r="A16" s="10" t="n">
         <v>44872</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="C16" s="8" t="inlineStr">
+      <c r="C16" s="9" t="inlineStr">
         <is>
           <t>persimmon</t>
         </is>
       </c>
-      <c r="D16" s="8" t="inlineStr">
+      <c r="D16" s="9" t="inlineStr">
         <is>
           <t>Iran</t>
         </is>
       </c>
-      <c r="E16" s="8" t="inlineStr">
+      <c r="E16" s="9" t="inlineStr">
         <is>
           <t>deep orange</t>
         </is>
       </c>
-      <c r="F16" s="9" t="n">
+      <c r="F16" t="n">
         <v>11</v>
       </c>
-      <c r="G16" s="9" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>persimmon</t>
         </is>
       </c>
-      <c r="H16" s="9" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>acorn</t>
         </is>
       </c>
-      <c r="I16" s="9" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>deep orange</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="12.8" customHeight="1" s="6">
+    <row r="17" ht="12.8" customHeight="1" s="7">
       <c r="A17" s="10" t="n">
         <v>44885</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="8" t="inlineStr">
+      <c r="C17" s="9" t="inlineStr">
         <is>
           <t>coconut</t>
         </is>
       </c>
-      <c r="D17" s="8" t="inlineStr">
+      <c r="D17" s="9" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="E17" s="8" t="inlineStr">
+      <c r="E17" s="9" t="inlineStr">
         <is>
           <t>brown</t>
         </is>
       </c>
-      <c r="F17" s="9" t="n"/>
-      <c r="G17" s="9" t="n"/>
-      <c r="H17" s="9" t="n"/>
-      <c r="I17" s="9" t="n"/>
-    </row>
-    <row r="18" ht="12.8" customHeight="1" s="6">
+      <c r="F17" s="11" t="n"/>
+      <c r="G17" s="11" t="n"/>
+      <c r="H17" s="11" t="n"/>
+      <c r="I17" s="11" t="n"/>
+    </row>
+    <row r="18" ht="12.8" customHeight="1" s="7">
       <c r="A18" s="10" t="n">
         <v>44886</v>
       </c>
-      <c r="B18" s="8" t="n">
+      <c r="B18" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C18" s="8" t="inlineStr">
+      <c r="C18" s="9" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="D18" s="8" t="inlineStr">
+      <c r="D18" s="9" t="inlineStr">
         <is>
           <t>Thailand</t>
         </is>
       </c>
-      <c r="E18" s="8" t="n"/>
-      <c r="F18" s="9" t="n">
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" t="n">
         <v>4</v>
       </c>
-      <c r="G18" s="9" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="H18" s="9" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>flat</t>
         </is>
       </c>
-      <c r="I18" s="9" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-      <c r="J18" s="8" t="n"/>
-    </row>
-    <row r="19" ht="12.8" customHeight="1" s="6">
-      <c r="J19" s="11" t="n"/>
-    </row>
-    <row r="20" ht="12.8" customHeight="1" s="6"/>
+    </row>
+    <row r="19" ht="12.8" customHeight="1" s="7"/>
+    <row r="20" ht="12.8" customHeight="1" s="7">
+      <c r="A20" s="9" t="inlineStr">
+        <is>
+          <t>Trailing row here</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>